<commit_message>
kind editor and attachments success
</commit_message>
<xml_diff>
--- a/.documents/功能进度计划.xlsx
+++ b/.documents/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="102">
   <si>
     <t>需求名称</t>
   </si>
@@ -255,221 +255,201 @@
     <t>待增加功能</t>
   </si>
   <si>
+    <t>icustom cloud</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题修复</t>
+  </si>
+  <si>
+    <t>取消</t>
+  </si>
+  <si>
+    <t>取消</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>载入Spring配置文件后Junit测试失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原测试正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待开发界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待数据接通</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源过滤器的拦截使页面 不兼容浏览器,源码被直接打印出来了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>各模块按条件查询功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前查询表单未继续进行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类似Google Advanced REST Client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发责任人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试责任人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aGuang</t>
+  </si>
+  <si>
+    <t>aGuang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试start pom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发start pom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">基本代码已经完成,需要再好好扩展,上传的类型,大小需要根据数据字典定义,下载的文件是写死的路径 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公共模板页调用国际化接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>切换国家时发送国际化参数,并调用国际化接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公共缓存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>富文本模块-通过URL替换CSS\HTML\JS等内容,不用重新发包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础组件开发</t>
+  </si>
+  <si>
+    <t>基础组件开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lookup 数据列表开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cxf  java配置方式多个模块的配置不能并存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>security 4 增加当前用户接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件管理,文件上传下载组件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写一个 JS分页插件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icustom metrics  监控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icustom.activiti 工作流开发，并且有demo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户角色管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色资源管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试功能开发</t>
+  </si>
+  <si>
+    <t>测试功能开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试功能开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂停</t>
+  </si>
+  <si>
+    <t>参考common.htmlarea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>子功能点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common.kindeditor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件上传</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符输入输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对输入的字符转义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>富文本编辑器在FF渲染有问题，替换内容过滤器还待开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>icustom redis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>icustom cloud</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题修复</t>
-  </si>
-  <si>
-    <t>取消</t>
-  </si>
-  <si>
-    <t>取消</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>载入Spring配置文件后Junit测试失败</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>原测试正常</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待开发界面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待数据接通</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 待应用到实际数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>资源过滤器的拦截使页面 不兼容浏览器,源码被直接打印出来了</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>各模块按条件查询功能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>当前查询表单未继续进行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>类似Google Advanced REST Client</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开发责任人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试责任人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>aGuang</t>
-  </si>
-  <si>
-    <t>aGuang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试start pom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开发start pom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">基本代码已经完成,需要再好好扩展,上传的类型,大小需要根据数据字典定义,下载的文件是写死的路径 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>公共模板页调用国际化接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>切换国家时发送国际化参数,并调用国际化接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>公共缓存</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>富文本模块-通过URL替换CSS\HTML\JS等内容,不用重新发包</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>基础组件开发</t>
-  </si>
-  <si>
-    <t>基础组件开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lookup 数据列表开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cxf  java配置方式多个模块的配置不能并存</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>security 4 增加当前用户接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>附件管理,文件上传下载组件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>写一个 JS分页插件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>icustom metrics  监控</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>icustom.activiti 工作流开发，并且有demo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>资源管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户角色管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色资源管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试功能开发</t>
-  </si>
-  <si>
-    <t>测试功能开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试功能开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">cxf security </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>暂停</t>
-  </si>
-  <si>
-    <t>参考common.htmlarea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>子功能点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>资源权限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>马上进行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>基础功能开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common.kindeditor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>附件上传</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符输入输出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对输入的字符转义</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>富文本编辑器在FF渲染有问题，替换内容过滤器还待开发</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -588,7 +568,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -648,37 +628,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,12 +713,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -795,6 +745,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1549,8 +1511,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L47" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:L47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L45" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:L45">
     <filterColumn colId="2"/>
     <filterColumn colId="4"/>
     <filterColumn colId="6"/>
@@ -1877,18 +1839,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" style="11"/>
     <col min="2" max="2" width="57.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5" style="37" customWidth="1"/>
+    <col min="3" max="3" width="57.5" style="35" customWidth="1"/>
     <col min="4" max="4" width="13.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
     <col min="6" max="9" width="13.25" style="1" customWidth="1"/>
@@ -1908,8 +1870,8 @@
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>98</v>
+      <c r="C1" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>1</v>
@@ -1921,10 +1883,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>30</v>
@@ -1946,17 +1908,17 @@
       <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="30"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>32</v>
@@ -1971,10 +1933,10 @@
         <v>6</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="24.75" customHeight="1">
@@ -1984,7 +1946,7 @@
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="30"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13" t="s">
         <v>20</v>
@@ -2005,10 +1967,10 @@
         <v>12</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="24.75" customHeight="1">
@@ -2018,7 +1980,7 @@
       <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
         <v>20</v>
@@ -2046,7 +2008,7 @@
       <c r="B5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
         <v>20</v>
@@ -2074,7 +2036,7 @@
       <c r="B6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
         <v>20</v>
@@ -2094,7 +2056,7 @@
         <v>16</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="24.75" customHeight="1">
@@ -2104,13 +2066,13 @@
       <c r="B7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="31"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -2124,7 +2086,7 @@
         <v>17</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="24.75" customHeight="1">
@@ -2134,7 +2096,7 @@
       <c r="B8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
         <v>8</v>
@@ -2150,7 +2112,7 @@
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O8" s="10" t="s">
         <v>21</v>
@@ -2163,13 +2125,13 @@
       <c r="B9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -2178,23 +2140,23 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="O9" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="24.75" customHeight="1">
-      <c r="A10" s="18">
+      <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="33"/>
+        <v>81</v>
+      </c>
+      <c r="C10" s="31"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -2202,7 +2164,7 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O10" s="9" t="s">
         <v>25</v>
@@ -2215,13 +2177,13 @@
       <c r="B11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -2234,13 +2196,13 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="24.75" customHeight="1">
-      <c r="A12" s="18">
+      <c r="A12" s="12">
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16" t="s">
         <v>26</v>
@@ -2262,13 +2224,13 @@
       <c r="B13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -2284,10 +2246,10 @@
       <c r="B14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -2304,10 +2266,10 @@
       <c r="B15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -2324,13 +2286,13 @@
       <c r="B16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="30"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -2344,9 +2306,9 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="30"/>
+        <v>82</v>
+      </c>
+      <c r="C17" s="28"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>28</v>
@@ -2368,7 +2330,7 @@
       <c r="B18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>9</v>
@@ -2390,7 +2352,7 @@
       <c r="B19" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="30"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13" t="s">
         <v>9</v>
@@ -2406,91 +2368,89 @@
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A20" s="18">
+      <c r="A20" s="12">
         <v>19</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="C20" s="32"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="24.75" customHeight="1">
       <c r="A21" s="12">
         <v>20</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13" t="s">
+      <c r="B21" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="F21" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A22" s="18">
+      <c r="A22" s="12">
         <v>21</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="B22" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
-      <c r="L22" s="13" t="s">
-        <v>58</v>
-      </c>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" ht="24.75" customHeight="1">
       <c r="A23" s="12">
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="30"/>
+        <v>46</v>
+      </c>
+      <c r="C23" s="28"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
@@ -2504,16 +2464,14 @@
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="C24" s="28"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>49</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
@@ -2526,9 +2484,9 @@
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="C25" s="28"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13" t="s">
         <v>28</v>
@@ -2546,104 +2504,104 @@
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="30"/>
+        <v>55</v>
+      </c>
+      <c r="C26" s="28"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
+      <c r="K26" s="25">
+        <v>43066</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A27" s="18">
+      <c r="A27" s="12">
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="30"/>
+        <v>59</v>
+      </c>
+      <c r="C27" s="28"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+        <v>52</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
-      <c r="K27" s="27">
-        <v>43066</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>97</v>
-      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" ht="24.75" customHeight="1">
       <c r="A28" s="12">
         <v>27</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="33"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" ht="24.75" customHeight="1">
       <c r="A29" s="12">
         <v>28</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="35"/>
+        <v>69</v>
+      </c>
+      <c r="C29" s="33"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>49</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
-      <c r="L29" s="21" t="s">
-        <v>63</v>
-      </c>
+      <c r="L29" s="21"/>
     </row>
     <row r="30" spans="1:12" ht="24.75" customHeight="1">
       <c r="A30" s="12">
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="35"/>
+        <v>70</v>
+      </c>
+      <c r="C30" s="33"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
@@ -2657,15 +2615,17 @@
       <c r="A31" s="12">
         <v>30</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="20"/>
+      <c r="B31" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="39"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>49</v>
+      </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
@@ -2677,46 +2637,48 @@
       <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20" t="s">
+      <c r="B32" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="39"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="20" t="s">
-        <v>49</v>
+      <c r="F32" s="38" t="s">
+        <v>50</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
       <c r="K32" s="20"/>
-      <c r="L32" s="21"/>
+      <c r="L32" s="21" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="24.75" customHeight="1">
       <c r="A33" s="12">
         <v>32</v>
       </c>
-      <c r="B33" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="21" t="s">
+      <c r="B33" s="19" t="s">
         <v>75</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="24.75" customHeight="1">
@@ -2724,42 +2686,40 @@
         <v>33</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="30"/>
+        <v>78</v>
+      </c>
+      <c r="C34" s="28"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
-      <c r="L34" s="13" t="s">
-        <v>106</v>
-      </c>
+      <c r="L34" s="24"/>
     </row>
     <row r="35" spans="1:12" ht="24.75" customHeight="1">
       <c r="A35" s="12">
         <v>34</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="30"/>
+        <v>79</v>
+      </c>
+      <c r="C35" s="28"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+        <v>12</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
@@ -2769,77 +2729,73 @@
       <c r="A36" s="12">
         <v>35</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>12</v>
+      <c r="B36" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="34"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="24"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="21"/>
     </row>
     <row r="37" spans="1:12" ht="24.75" customHeight="1">
       <c r="A37" s="12">
         <v>36</v>
       </c>
-      <c r="B37" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>49</v>
-      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="21"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="24"/>
     </row>
     <row r="38" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A38" s="26"/>
-      <c r="B38" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13" t="s">
+      <c r="A38" s="12">
+        <v>37</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="37"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="36" t="s">
         <v>49</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="24"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="21"/>
     </row>
     <row r="39" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A39" s="25">
-        <v>37</v>
+      <c r="A39" s="12">
+        <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="35"/>
+        <v>85</v>
+      </c>
+      <c r="C39" s="33"/>
       <c r="D39" s="20"/>
       <c r="E39" s="20" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F39" s="20" t="s">
         <v>49</v>
@@ -2852,13 +2808,13 @@
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A40" s="25">
-        <v>38</v>
+      <c r="A40" s="12">
+        <v>39</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="35"/>
+        <v>86</v>
+      </c>
+      <c r="C40" s="33"/>
       <c r="D40" s="20"/>
       <c r="E40" s="20" t="s">
         <v>9</v>
@@ -2874,13 +2830,13 @@
       <c r="L40" s="21"/>
     </row>
     <row r="41" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A41" s="25">
-        <v>39</v>
+      <c r="A41" s="12">
+        <v>40</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="35"/>
+        <v>87</v>
+      </c>
+      <c r="C41" s="33"/>
       <c r="D41" s="20"/>
       <c r="E41" s="20" t="s">
         <v>9</v>
@@ -2896,13 +2852,13 @@
       <c r="L41" s="21"/>
     </row>
     <row r="42" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A42" s="25">
-        <v>40</v>
+      <c r="A42" s="12">
+        <v>41</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" s="35"/>
+        <v>88</v>
+      </c>
+      <c r="C42" s="33"/>
       <c r="D42" s="20"/>
       <c r="E42" s="20" t="s">
         <v>9</v>
@@ -2918,13 +2874,13 @@
       <c r="L42" s="21"/>
     </row>
     <row r="43" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A43" s="25">
-        <v>41</v>
+      <c r="A43" s="12">
+        <v>42</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="35"/>
+        <v>89</v>
+      </c>
+      <c r="C43" s="33"/>
       <c r="D43" s="20"/>
       <c r="E43" s="20" t="s">
         <v>9</v>
@@ -2940,83 +2896,43 @@
       <c r="L43" s="21"/>
     </row>
     <row r="44" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A44" s="25">
-        <v>42</v>
+      <c r="A44" s="12">
+        <v>43</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="35"/>
+        <v>96</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>97</v>
+      </c>
       <c r="D44" s="20"/>
       <c r="E44" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>49</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F44" s="20"/>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
-      <c r="L44" s="21"/>
+      <c r="L44" s="20"/>
     </row>
     <row r="45" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A45" s="20">
-        <v>43</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="20"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="D45" s="20"/>
-      <c r="E45" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>101</v>
-      </c>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
       <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-    </row>
-    <row r="46" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20"/>
-    </row>
-    <row r="47" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20" t="s">
-        <v>105</v>
+      <c r="L45" s="20" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3102,7 +3018,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -3116,20 +3032,20 @@
         <v>26</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.5">
@@ -3137,14 +3053,14 @@
         <v>27</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>

</xml_diff>

<commit_message>
user and role test case
</commit_message>
<xml_diff>
--- a/.documents/功能进度计划.xlsx
+++ b/.documents/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="102">
   <si>
     <t>需求名称</t>
   </si>
@@ -367,89 +367,89 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>附件管理,文件上传下载组件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写一个 JS分页插件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icustom metrics  监控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icustom.activiti 工作流开发，并且有demo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户角色管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色资源管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试功能开发</t>
+  </si>
+  <si>
+    <t>测试功能开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试功能开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂停</t>
+  </si>
+  <si>
+    <t>参考common.htmlarea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>子功能点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common.kindeditor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件上传</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>富文本编辑器在FF渲染有问题，替换内容过滤器还待开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icustom redis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>security 4 增加当前用户接口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>附件管理,文件上传下载组件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>写一个 JS分页插件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>icustom metrics  监控</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>icustom.activiti 工作流开发，并且有demo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>资源管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户角色管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色资源管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试功能开发</t>
-  </si>
-  <si>
-    <t>测试功能开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试功能开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>暂停</t>
-  </si>
-  <si>
-    <t>参考common.htmlarea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>子功能点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common.kindeditor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>附件上传</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符输入输出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对输入的字符转义</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>富文本编辑器在FF渲染有问题，替换内容过滤器还待开发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>icustom redis</t>
+    <t>完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件上传下载demo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -568,7 +568,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -628,13 +628,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -716,9 +729,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -735,15 +745,9 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -758,6 +762,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1511,8 +1518,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L45" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:L45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L44" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:L44">
     <filterColumn colId="2"/>
     <filterColumn colId="4"/>
     <filterColumn colId="6"/>
@@ -1839,18 +1846,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" style="11"/>
     <col min="2" max="2" width="57.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5" style="35" customWidth="1"/>
+    <col min="3" max="3" width="57.5" style="32" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
     <col min="6" max="9" width="13.25" style="1" customWidth="1"/>
@@ -1870,8 +1877,8 @@
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>95</v>
+      <c r="C1" s="26" t="s">
+        <v>94</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>1</v>
@@ -1908,7 +1915,7 @@
       <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13" t="s">
         <v>20</v>
@@ -1946,7 +1953,7 @@
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13" t="s">
         <v>20</v>
@@ -1980,7 +1987,7 @@
       <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
         <v>20</v>
@@ -2008,7 +2015,7 @@
       <c r="B5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
         <v>20</v>
@@ -2036,7 +2043,7 @@
       <c r="B6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
         <v>20</v>
@@ -2066,7 +2073,7 @@
       <c r="B7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="29"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22" t="s">
         <v>20</v>
@@ -2086,7 +2093,7 @@
         <v>17</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="24.75" customHeight="1">
@@ -2096,7 +2103,7 @@
       <c r="B8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
         <v>8</v>
@@ -2125,13 +2132,13 @@
       <c r="B9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -2147,16 +2154,16 @@
       <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>76</v>
+      <c r="B10" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -2177,7 +2184,7 @@
       <c r="B11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
         <v>20</v>
@@ -2202,7 +2209,7 @@
       <c r="B12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="31"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16" t="s">
         <v>26</v>
@@ -2224,13 +2231,13 @@
       <c r="B13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -2246,7 +2253,7 @@
       <c r="B14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>53</v>
@@ -2266,7 +2273,7 @@
       <c r="B15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>53</v>
@@ -2286,7 +2293,7 @@
       <c r="B16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>20</v>
@@ -2306,9 +2313,9 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="28"/>
+        <v>81</v>
+      </c>
+      <c r="C17" s="27"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>28</v>
@@ -2330,7 +2337,7 @@
       <c r="B18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>9</v>
@@ -2352,7 +2359,7 @@
       <c r="B19" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="28"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13" t="s">
         <v>9</v>
@@ -2371,12 +2378,12 @@
       <c r="A20" s="12">
         <v>19</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19" t="s">
+      <c r="B20" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="s">
         <v>28</v>
       </c>
       <c r="F20" s="19" t="s">
@@ -2395,12 +2402,12 @@
       <c r="A21" s="12">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19" t="s">
+      <c r="B21" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="19" t="s">
@@ -2420,9 +2427,9 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="28"/>
+        <v>83</v>
+      </c>
+      <c r="C22" s="27"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13" t="s">
         <v>9</v>
@@ -2444,7 +2451,7 @@
       <c r="B23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13" t="s">
         <v>9</v>
@@ -2466,7 +2473,7 @@
       <c r="B24" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="28"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13" t="s">
         <v>28</v>
@@ -2486,7 +2493,7 @@
       <c r="B25" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13" t="s">
         <v>28</v>
@@ -2506,7 +2513,7 @@
       <c r="B26" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="28"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
         <v>20</v>
@@ -2522,7 +2529,7 @@
         <v>43066</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="24.75" customHeight="1">
@@ -2532,7 +2539,7 @@
       <c r="B27" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="28"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13" t="s">
         <v>20</v>
@@ -2554,7 +2561,7 @@
       <c r="B28" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="33"/>
+      <c r="C28" s="31"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20" t="s">
         <v>28</v>
@@ -2578,7 +2585,7 @@
       <c r="B29" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="33"/>
+      <c r="C29" s="31"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20" t="s">
         <v>53</v>
@@ -2598,7 +2605,7 @@
       <c r="B30" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="33"/>
+      <c r="C30" s="31"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20" t="s">
         <v>20</v>
@@ -2615,15 +2622,15 @@
       <c r="A31" s="12">
         <v>30</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="38" t="s">
+      <c r="F31" s="35" t="s">
         <v>49</v>
       </c>
       <c r="G31" s="20"/>
@@ -2637,15 +2644,15 @@
       <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38" t="s">
+      <c r="C32" s="34"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="38" t="s">
+      <c r="F32" s="35" t="s">
         <v>50</v>
       </c>
       <c r="G32" s="20"/>
@@ -2661,12 +2668,12 @@
       <c r="A33" s="12">
         <v>32</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19" t="s">
+      <c r="C33" s="30"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="19" t="s">
@@ -2678,7 +2685,7 @@
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="24.75" customHeight="1">
@@ -2688,7 +2695,7 @@
       <c r="B34" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="28"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13" t="s">
         <v>20</v>
@@ -2710,10 +2717,10 @@
       <c r="B35" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F35" s="13" t="s">
         <v>12</v>
@@ -2729,13 +2736,13 @@
       <c r="A36" s="12">
         <v>35</v>
       </c>
-      <c r="B36" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="16" t="s">
-        <v>20</v>
+      <c r="B36" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>49</v>
@@ -2749,33 +2756,39 @@
     </row>
     <row r="37" spans="1:12" ht="24.75" customHeight="1">
       <c r="A37" s="12">
-        <v>36</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+        <v>37</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>49</v>
+      </c>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="24"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="21"/>
     </row>
     <row r="38" spans="1:12" ht="24.75" customHeight="1">
       <c r="A38" s="12">
-        <v>37</v>
-      </c>
-      <c r="B38" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="36" t="s">
+      <c r="F38" s="20" t="s">
         <v>49</v>
       </c>
       <c r="G38" s="20"/>
@@ -2787,14 +2800,14 @@
     </row>
     <row r="39" spans="1:12" ht="24.75" customHeight="1">
       <c r="A39" s="12">
-        <v>38</v>
-      </c>
-      <c r="B39" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="33"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20" t="s">
+      <c r="C39" s="36"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35" t="s">
         <v>9</v>
       </c>
       <c r="F39" s="20" t="s">
@@ -2809,14 +2822,14 @@
     </row>
     <row r="40" spans="1:12" ht="24.75" customHeight="1">
       <c r="A40" s="12">
-        <v>39</v>
-      </c>
-      <c r="B40" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20" t="s">
+      <c r="C40" s="36"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="20" t="s">
@@ -2831,14 +2844,14 @@
     </row>
     <row r="41" spans="1:12" ht="24.75" customHeight="1">
       <c r="A41" s="12">
-        <v>40</v>
-      </c>
-      <c r="B41" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="33"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20" t="s">
+      <c r="C41" s="36"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35" t="s">
         <v>9</v>
       </c>
       <c r="F41" s="20" t="s">
@@ -2853,14 +2866,14 @@
     </row>
     <row r="42" spans="1:12" ht="24.75" customHeight="1">
       <c r="A42" s="12">
-        <v>41</v>
-      </c>
-      <c r="B42" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20" t="s">
+      <c r="C42" s="36"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35" t="s">
         <v>9</v>
       </c>
       <c r="F42" s="20" t="s">
@@ -2875,65 +2888,47 @@
     </row>
     <row r="43" spans="1:12" ht="24.75" customHeight="1">
       <c r="A43" s="12">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="33"/>
+        <v>95</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>96</v>
+      </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
-      <c r="L43" s="21"/>
+      <c r="L43" s="20"/>
     </row>
     <row r="44" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A44" s="12">
-        <v>43</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="20"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="31"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-    </row>
-    <row r="45" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20" t="s">
-        <v>99</v>
-      </c>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
excel import and export successful
</commit_message>
<xml_diff>
--- a/.documents/功能进度计划.xlsx
+++ b/.documents/功能进度计划.xlsx
@@ -568,7 +568,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -591,63 +591,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -711,19 +661,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
@@ -745,32 +686,397 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1108,376 +1414,6 @@
         <name val="微软雅黑"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1526,36 +1462,36 @@
     <filterColumn colId="7"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="序列" dataDxfId="22"/>
-    <tableColumn id="2" name="需求名称" dataDxfId="21"/>
-    <tableColumn id="12" name="子功能点" dataDxfId="20"/>
-    <tableColumn id="3" name="优先级别" dataDxfId="19"/>
-    <tableColumn id="4" name="完成状态" dataDxfId="18"/>
-    <tableColumn id="5" name="计划类型" dataDxfId="17"/>
-    <tableColumn id="10" name="开发" dataDxfId="16"/>
-    <tableColumn id="11" name="测试" dataDxfId="15"/>
-    <tableColumn id="6" name="功能维度" dataDxfId="14"/>
-    <tableColumn id="7" name="计划日期" dataDxfId="13"/>
-    <tableColumn id="8" name="完成日期" dataDxfId="12"/>
-    <tableColumn id="9" name="补充说明" dataDxfId="11"/>
+    <tableColumn id="1" name="序列" dataDxfId="11"/>
+    <tableColumn id="2" name="需求名称" dataDxfId="10"/>
+    <tableColumn id="12" name="子功能点" dataDxfId="9"/>
+    <tableColumn id="3" name="优先级别" dataDxfId="8"/>
+    <tableColumn id="4" name="完成状态" dataDxfId="7"/>
+    <tableColumn id="5" name="计划类型" dataDxfId="6"/>
+    <tableColumn id="10" name="开发" dataDxfId="5"/>
+    <tableColumn id="11" name="测试" dataDxfId="4"/>
+    <tableColumn id="6" name="功能维度" dataDxfId="3"/>
+    <tableColumn id="7" name="计划日期" dataDxfId="2"/>
+    <tableColumn id="8" name="完成日期" dataDxfId="1"/>
+    <tableColumn id="9" name="补充说明" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:I4"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="序列" dataDxfId="8"/>
-    <tableColumn id="2" name="需求名称" dataDxfId="7"/>
-    <tableColumn id="3" name="优先级别" dataDxfId="6"/>
-    <tableColumn id="4" name="完成状态" dataDxfId="5"/>
-    <tableColumn id="5" name="计划类型" dataDxfId="4"/>
-    <tableColumn id="6" name="功能维度" dataDxfId="3"/>
-    <tableColumn id="7" name="计划日期" dataDxfId="2"/>
-    <tableColumn id="8" name="完成日期" dataDxfId="1"/>
-    <tableColumn id="9" name="补充说明" dataDxfId="0"/>
+    <tableColumn id="1" name="序列" dataDxfId="20"/>
+    <tableColumn id="2" name="需求名称" dataDxfId="19"/>
+    <tableColumn id="3" name="优先级别" dataDxfId="18"/>
+    <tableColumn id="4" name="完成状态" dataDxfId="17"/>
+    <tableColumn id="5" name="计划类型" dataDxfId="16"/>
+    <tableColumn id="6" name="功能维度" dataDxfId="15"/>
+    <tableColumn id="7" name="计划日期" dataDxfId="14"/>
+    <tableColumn id="8" name="完成日期" dataDxfId="13"/>
+    <tableColumn id="9" name="补充说明" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1849,15 +1785,15 @@
   <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44:F44"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" style="11"/>
     <col min="2" max="2" width="57.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5" style="32" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="57.5" style="28" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
     <col min="6" max="9" width="13.25" style="1" customWidth="1"/>
@@ -1877,7 +1813,7 @@
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>94</v>
       </c>
       <c r="D1" s="15" t="s">
@@ -1915,7 +1851,7 @@
       <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13" t="s">
         <v>20</v>
@@ -1953,7 +1889,7 @@
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13" t="s">
         <v>20</v>
@@ -1987,7 +1923,7 @@
       <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
         <v>20</v>
@@ -2015,7 +1951,7 @@
       <c r="B5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
         <v>20</v>
@@ -2043,7 +1979,7 @@
       <c r="B6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
         <v>20</v>
@@ -2070,12 +2006,12 @@
       <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="13" t="s">
@@ -2100,15 +2036,15 @@
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="23" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="13"/>
@@ -2118,7 +2054,7 @@
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="13" t="s">
         <v>62</v>
       </c>
       <c r="O8" s="10" t="s">
@@ -2132,10 +2068,10 @@
       <c r="B9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>89</v>
@@ -2184,7 +2120,7 @@
       <c r="B11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
         <v>20</v>
@@ -2209,7 +2145,7 @@
       <c r="B12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16" t="s">
         <v>26</v>
@@ -2231,7 +2167,7 @@
       <c r="B13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
         <v>14</v>
@@ -2253,7 +2189,7 @@
       <c r="B14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="27"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>53</v>
@@ -2273,7 +2209,7 @@
       <c r="B15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>53</v>
@@ -2293,7 +2229,7 @@
       <c r="B16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>20</v>
@@ -2315,7 +2251,7 @@
       <c r="B17" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>28</v>
@@ -2337,7 +2273,7 @@
       <c r="B18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="27"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>9</v>
@@ -2359,7 +2295,7 @@
       <c r="B19" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13" t="s">
         <v>9</v>
@@ -2381,10 +2317,10 @@
       <c r="B20" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="30"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>49</v>
@@ -2405,10 +2341,10 @@
       <c r="B21" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F21" s="19" t="s">
         <v>76</v>
@@ -2429,7 +2365,7 @@
       <c r="B22" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13" t="s">
         <v>9</v>
@@ -2451,7 +2387,7 @@
       <c r="B23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13" t="s">
         <v>9</v>
@@ -2473,7 +2409,7 @@
       <c r="B24" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="27"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13" t="s">
         <v>28</v>
@@ -2493,7 +2429,7 @@
       <c r="B25" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="27"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13" t="s">
         <v>28</v>
@@ -2513,7 +2449,7 @@
       <c r="B26" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="27"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
         <v>20</v>
@@ -2525,7 +2461,7 @@
       <c r="H26" s="19"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
-      <c r="K26" s="25">
+      <c r="K26" s="22">
         <v>43066</v>
       </c>
       <c r="L26" s="13" t="s">
@@ -2539,7 +2475,7 @@
       <c r="B27" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="27"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13" t="s">
         <v>20</v>
@@ -2558,23 +2494,23 @@
       <c r="A28" s="12">
         <v>27</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20" t="s">
+      <c r="C28" s="24"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="21" t="s">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2582,85 +2518,85 @@
       <c r="A29" s="12">
         <v>28</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20" t="s">
+      <c r="C29" s="24"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="21"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" ht="24.75" customHeight="1">
       <c r="A30" s="12">
         <v>29</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20" t="s">
+      <c r="C30" s="24"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="21"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" ht="24.75" customHeight="1">
       <c r="A31" s="12">
         <v>30</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33" t="s">
+      <c r="C31" s="27"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="21"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" ht="24.75" customHeight="1">
       <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33" t="s">
+      <c r="C32" s="27"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="35" t="s">
+      <c r="F32" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="21" t="s">
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2671,7 +2607,7 @@
       <c r="B33" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="30"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="16"/>
       <c r="E33" s="16" t="s">
         <v>8</v>
@@ -2695,7 +2631,7 @@
       <c r="B34" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="27"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13" t="s">
         <v>20</v>
@@ -2708,7 +2644,7 @@
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
-      <c r="L34" s="24"/>
+      <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="24.75" customHeight="1">
       <c r="A35" s="12">
@@ -2717,7 +2653,7 @@
       <c r="B35" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="27"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13" t="s">
         <v>92</v>
@@ -2725,12 +2661,12 @@
       <c r="F35" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
-      <c r="L35" s="24"/>
+      <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="24.75" customHeight="1">
       <c r="A36" s="12">
@@ -2744,178 +2680,178 @@
       <c r="E36" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="21"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="24.75" customHeight="1">
       <c r="A37" s="12">
         <v>37</v>
       </c>
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33" t="s">
+      <c r="C37" s="27"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="33" t="s">
+      <c r="F37" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="21"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="24.75" customHeight="1">
       <c r="A38" s="12">
         <v>38</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35" t="s">
+      <c r="C38" s="29"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="21"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="24.75" customHeight="1">
       <c r="A39" s="12">
         <v>39</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35" t="s">
+      <c r="C39" s="29"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="21"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="24.75" customHeight="1">
       <c r="A40" s="12">
         <v>40</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35" t="s">
+      <c r="C40" s="29"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="21"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="24.75" customHeight="1">
       <c r="A41" s="12">
         <v>41</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="36"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35" t="s">
+      <c r="C41" s="29"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="21"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="24.75" customHeight="1">
       <c r="A42" s="12">
         <v>42</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="36"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35" t="s">
+      <c r="C42" s="29"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="21"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="24.75" customHeight="1">
       <c r="A43" s="12">
         <v>43</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20" t="s">
+      <c r="D43" s="13"/>
+      <c r="E43" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A44" s="37"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="31"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13" t="s">
         <v>28</v>
@@ -2923,12 +2859,12 @@
       <c r="F44" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
-      <c r="L44" s="24"/>
+      <c r="L44" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
html area api test case start
</commit_message>
<xml_diff>
--- a/.documents/功能进度计划.xlsx
+++ b/.documents/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="117">
   <si>
     <t>需求名称</t>
   </si>
@@ -450,6 +450,63 @@
   </si>
   <si>
     <t>附件上传下载demo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用 Docker 构建、运行、发布一个 Spring Boot 应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定时任务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快速开发模板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码生成工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础环境功能</t>
+  </si>
+  <si>
+    <t>基础环境功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相关设计工作</t>
+  </si>
+  <si>
+    <t>相关设计工作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部署功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>监控与告警功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日志聚合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国际化、数据字典、权限管理api编写api测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>富文本模块-API测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能测试</t>
+  </si>
+  <si>
+    <t>功能测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -568,7 +625,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -591,13 +648,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -691,392 +761,21 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1414,6 +1113,386 @@
         <name val="微软雅黑"/>
         <scheme val="none"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1454,44 +1533,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L44" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:L44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L50" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:L50">
     <filterColumn colId="2"/>
     <filterColumn colId="4"/>
     <filterColumn colId="6"/>
     <filterColumn colId="7"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="序列" dataDxfId="11"/>
-    <tableColumn id="2" name="需求名称" dataDxfId="10"/>
-    <tableColumn id="12" name="子功能点" dataDxfId="9"/>
-    <tableColumn id="3" name="优先级别" dataDxfId="8"/>
-    <tableColumn id="4" name="完成状态" dataDxfId="7"/>
-    <tableColumn id="5" name="计划类型" dataDxfId="6"/>
-    <tableColumn id="10" name="开发" dataDxfId="5"/>
-    <tableColumn id="11" name="测试" dataDxfId="4"/>
-    <tableColumn id="6" name="功能维度" dataDxfId="3"/>
-    <tableColumn id="7" name="计划日期" dataDxfId="2"/>
-    <tableColumn id="8" name="完成日期" dataDxfId="1"/>
-    <tableColumn id="9" name="补充说明" dataDxfId="0"/>
+    <tableColumn id="1" name="序列" dataDxfId="22"/>
+    <tableColumn id="2" name="需求名称" dataDxfId="21"/>
+    <tableColumn id="12" name="子功能点" dataDxfId="20"/>
+    <tableColumn id="3" name="优先级别" dataDxfId="19"/>
+    <tableColumn id="4" name="完成状态" dataDxfId="18"/>
+    <tableColumn id="5" name="计划类型" dataDxfId="17"/>
+    <tableColumn id="10" name="开发" dataDxfId="16"/>
+    <tableColumn id="11" name="测试" dataDxfId="15"/>
+    <tableColumn id="6" name="功能维度" dataDxfId="14"/>
+    <tableColumn id="7" name="计划日期" dataDxfId="13"/>
+    <tableColumn id="8" name="完成日期" dataDxfId="12"/>
+    <tableColumn id="9" name="补充说明" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I4"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="序列" dataDxfId="20"/>
-    <tableColumn id="2" name="需求名称" dataDxfId="19"/>
-    <tableColumn id="3" name="优先级别" dataDxfId="18"/>
-    <tableColumn id="4" name="完成状态" dataDxfId="17"/>
-    <tableColumn id="5" name="计划类型" dataDxfId="16"/>
-    <tableColumn id="6" name="功能维度" dataDxfId="15"/>
-    <tableColumn id="7" name="计划日期" dataDxfId="14"/>
-    <tableColumn id="8" name="完成日期" dataDxfId="13"/>
-    <tableColumn id="9" name="补充说明" dataDxfId="12"/>
+    <tableColumn id="1" name="序列" dataDxfId="8"/>
+    <tableColumn id="2" name="需求名称" dataDxfId="7"/>
+    <tableColumn id="3" name="优先级别" dataDxfId="6"/>
+    <tableColumn id="4" name="完成状态" dataDxfId="5"/>
+    <tableColumn id="5" name="计划类型" dataDxfId="4"/>
+    <tableColumn id="6" name="功能维度" dataDxfId="3"/>
+    <tableColumn id="7" name="计划日期" dataDxfId="2"/>
+    <tableColumn id="8" name="完成日期" dataDxfId="1"/>
+    <tableColumn id="9" name="补充说明" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1782,11 +1861,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
@@ -1794,7 +1873,7 @@
     <col min="1" max="1" width="9" style="11"/>
     <col min="2" max="2" width="57.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="57.5" style="28" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
     <col min="6" max="9" width="13.25" style="1" customWidth="1"/>
     <col min="10" max="10" width="15" style="1" customWidth="1"/>
@@ -1856,7 +1935,9 @@
       <c r="E2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="13" t="s">
+        <v>106</v>
+      </c>
       <c r="G2" s="13" t="s">
         <v>67</v>
       </c>
@@ -1894,7 +1975,9 @@
       <c r="E3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="13"/>
+      <c r="F3" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
@@ -1928,7 +2011,9 @@
       <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="13"/>
+      <c r="F4" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="s">
@@ -1956,7 +2041,9 @@
       <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13" t="s">
@@ -2059,6 +2146,9 @@
       </c>
       <c r="O8" s="10" t="s">
         <v>21</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="24.75" customHeight="1">
@@ -2085,6 +2175,9 @@
       <c r="O9" s="10" t="s">
         <v>54</v>
       </c>
+      <c r="Q9" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10" spans="1:19" ht="24.75" customHeight="1">
       <c r="A10" s="12">
@@ -2106,11 +2199,14 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="17" t="s">
         <v>71</v>
       </c>
       <c r="O10" s="9" t="s">
         <v>25</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="24.75" customHeight="1">
@@ -2137,6 +2233,9 @@
       <c r="O11" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="Q11" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="12" spans="1:19" ht="24.75" customHeight="1">
       <c r="A12" s="12">
@@ -2159,6 +2258,9 @@
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
+      <c r="Q12" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:19" ht="24.75" customHeight="1">
       <c r="A13" s="12">
@@ -2181,6 +2283,9 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
+      <c r="Q13" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="14" spans="1:19" ht="24.75" customHeight="1">
       <c r="A14" s="12">
@@ -2414,7 +2519,9 @@
       <c r="E24" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="13"/>
+      <c r="F24" s="13" t="s">
+        <v>108</v>
+      </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
@@ -2434,7 +2541,9 @@
       <c r="E25" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="13"/>
+      <c r="F25" s="13" t="s">
+        <v>108</v>
+      </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
@@ -2524,9 +2633,11 @@
       <c r="C29" s="24"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
@@ -2546,7 +2657,9 @@
       <c r="E30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="13"/>
+      <c r="F30" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
@@ -2625,19 +2738,17 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A34" s="12">
-        <v>33</v>
-      </c>
+      <c r="A34" s="12"/>
       <c r="B34" s="13" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
@@ -2648,18 +2759,18 @@
     </row>
     <row r="35" spans="1:12" ht="24.75" customHeight="1">
       <c r="A35" s="12">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2670,18 +2781,18 @@
     </row>
     <row r="36" spans="1:12" ht="24.75" customHeight="1">
       <c r="A36" s="12">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="13"/>
+        <v>79</v>
+      </c>
+      <c r="C36" s="24"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
@@ -2692,17 +2803,17 @@
     </row>
     <row r="37" spans="1:12" ht="24.75" customHeight="1">
       <c r="A37" s="12">
-        <v>37</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F37" s="13" t="s">
         <v>49</v>
       </c>
       <c r="G37" s="13"/>
@@ -2714,17 +2825,17 @@
     </row>
     <row r="38" spans="1:12" ht="24.75" customHeight="1">
       <c r="A38" s="12">
-        <v>38</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="16" t="s">
         <v>49</v>
       </c>
       <c r="G38" s="13"/>
@@ -2736,10 +2847,10 @@
     </row>
     <row r="39" spans="1:12" ht="24.75" customHeight="1">
       <c r="A39" s="12">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="29"/>
       <c r="D39" s="19"/>
@@ -2758,10 +2869,10 @@
     </row>
     <row r="40" spans="1:12" ht="24.75" customHeight="1">
       <c r="A40" s="12">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C40" s="29"/>
       <c r="D40" s="19"/>
@@ -2780,10 +2891,10 @@
     </row>
     <row r="41" spans="1:12" ht="24.75" customHeight="1">
       <c r="A41" s="12">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" s="29"/>
       <c r="D41" s="19"/>
@@ -2802,10 +2913,10 @@
     </row>
     <row r="42" spans="1:12" ht="24.75" customHeight="1">
       <c r="A42" s="12">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="19"/>
@@ -2824,20 +2935,18 @@
     </row>
     <row r="43" spans="1:12" ht="24.75" customHeight="1">
       <c r="A43" s="12">
-        <v>43</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
@@ -2847,14 +2956,18 @@
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A44" s="12"/>
+      <c r="A44" s="12">
+        <v>42</v>
+      </c>
       <c r="B44" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="24"/>
+        <v>95</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>96</v>
+      </c>
       <c r="D44" s="13"/>
       <c r="E44" s="13" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>76</v>
@@ -2866,11 +2979,141 @@
       <c r="K44" s="13"/>
       <c r="L44" s="13"/>
     </row>
+    <row r="45" spans="1:12" ht="24.75" customHeight="1">
+      <c r="A45" s="12">
+        <v>43</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="24"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+    </row>
+    <row r="46" spans="1:12" ht="24.75" customHeight="1">
+      <c r="A46" s="12">
+        <v>44</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="31"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+    </row>
+    <row r="47" spans="1:12" ht="24.75" customHeight="1">
+      <c r="A47" s="12">
+        <v>45</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="31"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
+      <c r="L47" s="30"/>
+    </row>
+    <row r="48" spans="1:12" ht="24.75" customHeight="1">
+      <c r="A48" s="12">
+        <v>46</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="31"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="30"/>
+    </row>
+    <row r="49" spans="1:12" ht="24.75" customHeight="1">
+      <c r="A49" s="12">
+        <v>47</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="31"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="30"/>
+      <c r="L49" s="30"/>
+    </row>
+    <row r="50" spans="1:12" ht="24.75" customHeight="1">
+      <c r="A50" s="32"/>
+      <c r="B50" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="31"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="30"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
-      <formula1>$Q$3:$Q$8</formula1>
+      <formula1>$Q$3:$Q$18</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>$O$3:$O$11</formula1>

</xml_diff>